<commit_message>
Cambios menores durante revision de proto_1 de SETI
en el esquematico se incluye la frecuencia del FPB del sensado de corriente
en la BRD se aumenta el ancho de la pista de resistencia del DAC
</commit_message>
<xml_diff>
--- a/05.PLANNING/Baseline Project-Plan - BATTERY.xlsx
+++ b/05.PLANNING/Baseline Project-Plan - BATTERY.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/05.PLANNING/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E6C884-924D-4D44-B2BD-CF0E750F9F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD276AC7-330B-1944-85BA-903626E17B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6780" yWindow="3800" windowWidth="26440" windowHeight="15440" xr2:uid="{6AA177C1-431F-5740-ACE8-C0F6BE0F8309}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Baseline" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,6 +104,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="7" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,7 +162,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -167,6 +173,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,7 +497,7 @@
   <dimension ref="C3:AB53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,271 +546,814 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="3:28" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>2</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>3</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>4</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>1</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>2</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>3</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <v>4</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>1</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="6">
         <v>2</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="6">
         <v>3</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="6">
         <v>4</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="6">
         <v>1</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>2</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4" s="6">
         <v>3</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="6">
         <v>4</v>
       </c>
-      <c r="U4" s="7">
+      <c r="U4" s="6">
         <v>1</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="6">
         <v>2</v>
       </c>
-      <c r="W4" s="7">
+      <c r="W4" s="6">
         <v>3</v>
       </c>
-      <c r="X4" s="7">
+      <c r="X4" s="6">
         <v>4</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="Y4" s="6">
         <v>1</v>
       </c>
-      <c r="Z4" s="7">
+      <c r="Z4" s="6">
         <v>2</v>
       </c>
-      <c r="AA4" s="7">
+      <c r="AA4" s="6">
         <v>3</v>
       </c>
-      <c r="AB4" s="7">
+      <c r="AB4" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>44886</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
     </row>
     <row r="6" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C6" s="6"/>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C7" s="6"/>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10">
+        <v>16</v>
+      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C8" s="6"/>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C9" s="6"/>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C10" s="6"/>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="10">
+        <v>2</v>
+      </c>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10">
+        <v>10</v>
+      </c>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="C11" s="6"/>
-      <c r="D11" s="9" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="5"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="10">
+        <v>18</v>
+      </c>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="D12" s="9"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="D13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="D14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
     </row>
     <row r="15" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="D15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
     </row>
     <row r="16" spans="3:28" x14ac:dyDescent="0.2">
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D32" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+    </row>
+    <row r="17" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+    </row>
+    <row r="18" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+    </row>
+    <row r="19" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+    </row>
+    <row r="20" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+    </row>
+    <row r="21" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+    </row>
+    <row r="22" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+    </row>
+    <row r="23" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="9"/>
+    </row>
+    <row r="24" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+    </row>
+    <row r="25" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+    </row>
+    <row r="26" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+    </row>
+    <row r="27" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="9"/>
+    </row>
+    <row r="28" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="4:28" x14ac:dyDescent="0.2">
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" s="9"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" s="9"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" s="9"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" s="9"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D37" s="9"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D38" s="9"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D39" s="9"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="9"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D41" s="9"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D42" s="9"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D43" s="9"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D44" s="9"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D45" s="9"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D46" s="9"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D47" s="9"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D48" s="9"/>
+      <c r="D48" s="8"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D49" s="9"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D50" s="9"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D51" s="9"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D52" s="9"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D53" s="9"/>
+      <c r="D53" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>